<commit_message>
added new strong tags to make SEO more effecient
</commit_message>
<xml_diff>
--- a/Documents/CASH PAYMENTS JOURNAL TEMPLATE.xlsx
+++ b/Documents/CASH PAYMENTS JOURNAL TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC915E6-CBB6-A34C-92D1-6618CCD28D8B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B95F260-25AB-0942-B946-0DD3A5167A2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{929004DF-ABB3-FC47-A7B1-08399A84CCAF}"/>
   </bookViews>
@@ -472,22 +472,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,7 +809,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B4" sqref="B4:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
trying to utilise typescript
</commit_message>
<xml_diff>
--- a/Documents/CASH PAYMENTS JOURNAL TEMPLATE.xlsx
+++ b/Documents/CASH PAYMENTS JOURNAL TEMPLATE.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B95F260-25AB-0942-B946-0DD3A5167A2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653DC491-B18B-9B4F-A7B7-2A7F3AA123FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{929004DF-ABB3-FC47-A7B1-08399A84CCAF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{929004DF-ABB3-FC47-A7B1-08399A84CCAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,16 +54,16 @@
     <t>Sundry accounts</t>
   </si>
   <si>
-    <t xml:space="preserve">CASH PAYMENTS JOURNAL OF </t>
-  </si>
-  <si>
-    <t>Trading stock</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
     <t>NAME: </t>
+  </si>
+  <si>
+    <t>CASH PAYMENTS JOURNAL OF Bobs Traders for March 2017</t>
+  </si>
+  <si>
+    <t>Creditors Control</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -489,6 +495,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,17 +819,17 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:K5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="6.83203125" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="6.83203125" customWidth="1"/>
@@ -852,7 +862,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -894,7 +904,7 @@
     <row r="4" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
@@ -953,10 +963,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I6" s="22" t="s">
         <v>6</v>
@@ -1005,9 +1015,9 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="10"/>
@@ -1026,10 +1036,10 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
       <c r="L9" s="1"/>
@@ -1048,9 +1058,9 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="1"/>
@@ -1068,10 +1078,10 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="1"/>
@@ -1089,10 +1099,10 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="1"/>
@@ -1131,10 +1141,10 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
       <c r="L14" s="1"/>

</xml_diff>